<commit_message>
Actualización de archivos Excel
</commit_message>
<xml_diff>
--- a/data/Individuals - Training.xlsx
+++ b/data/Individuals - Training.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alberto/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527DAE79-1E09-5747-B4A3-ADFE024C5E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327D964E-92BC-174C-B3D7-905665279F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20020" xr2:uid="{A2D0A931-C5F6-EF44-8E19-3B892526D62A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="301">
   <si>
     <t>Ryan Andrews</t>
   </si>
@@ -930,6 +930,15 @@
   </si>
   <si>
     <t>INDIVIDUAL TECHNIQUE LONG BALL</t>
+  </si>
+  <si>
+    <t>SPECIFIC LINE DEFENSIVE</t>
+  </si>
+  <si>
+    <t>FINISHING PATTERNS</t>
+  </si>
+  <si>
+    <t>POSITIONING.PLAY IN THE POCKET</t>
   </si>
 </sst>
 </file>
@@ -1319,10 +1328,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D1F4C8-8FC1-6D4C-8100-17BA8EC0B4E7}">
-  <dimension ref="A1:F700"/>
+  <dimension ref="A1:F722"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A662" workbookViewId="0">
-      <selection activeCell="C704" sqref="C704"/>
+    <sheetView tabSelected="1" topLeftCell="A707" workbookViewId="0">
+      <selection activeCell="D725" sqref="D725"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9182,6 +9191,248 @@
         <v>292</v>
       </c>
     </row>
+    <row r="701" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A701" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B701" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C701" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="702" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A702" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B702" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C702" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="703" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A703" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B703" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C703" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="704" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A704" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B704" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C704" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="705" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A705" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B705" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C705" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="706" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A706" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B706" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C706" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="707" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A707" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B707" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C707" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="708" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A708" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B708" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C708" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="709" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A709" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B709" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C709" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="710" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A710" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B710" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C710" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="711" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A711" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B711" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C711" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="712" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A712" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B712" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C712" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="713" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A713" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B713" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C713" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="714" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A714" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B714" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C714" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="715" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A715" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B715" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C715" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="716" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A716" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B716" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C716" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="717" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A717" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B717" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C717" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="718" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A718" s="1">
+        <v>45944</v>
+      </c>
+      <c r="B718" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E718" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="719" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A719" s="1">
+        <v>45944</v>
+      </c>
+      <c r="B719" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C719" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="720" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A720" s="1">
+        <v>45944</v>
+      </c>
+      <c r="B720" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C720" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="721" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A721" s="1">
+        <v>45944</v>
+      </c>
+      <c r="B721" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C721" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="722" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A722" s="1">
+        <v>45944</v>
+      </c>
+      <c r="B722" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C722" t="s">
+        <v>288</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Ignorar archivo de datos Excel
</commit_message>
<xml_diff>
--- a/data/Individuals - Training.xlsx
+++ b/data/Individuals - Training.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alberto/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327D964E-92BC-174C-B3D7-905665279F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE551BC-7078-1D4D-82A1-97E44FAABE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20020" xr2:uid="{A2D0A931-C5F6-EF44-8E19-3B892526D62A}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="20000" xr2:uid="{A2D0A931-C5F6-EF44-8E19-3B892526D62A}"/>
   </bookViews>
   <sheets>
     <sheet name="Training individuales" sheetId="19" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="321">
   <si>
     <t>Ryan Andrews</t>
   </si>
@@ -939,6 +939,66 @@
   </si>
   <si>
     <t>POSITIONING.PLAY IN THE POCKET</t>
+  </si>
+  <si>
+    <t>REACTIONS SHOT &amp; FINISHING</t>
+  </si>
+  <si>
+    <t>FINISHING TWO TOUCHES COMPETITION</t>
+  </si>
+  <si>
+    <t>PROTECT SPACE &amp; MOVEMENT TO FINISHING</t>
+  </si>
+  <si>
+    <t>IMPROVING LONG BALL (LEFT FOOT)</t>
+  </si>
+  <si>
+    <t>BODY SHAPE &amp; LONG PASS</t>
+  </si>
+  <si>
+    <t>PENETRATE RUN &amp; FINISHING</t>
+  </si>
+  <si>
+    <t>BUILD UP &amp; IMPROVING LEFT FOOT</t>
+  </si>
+  <si>
+    <t>OPPONENT PRESS</t>
+  </si>
+  <si>
+    <t>POSITIONING GAME. PLAY FORWARD. DIFERENT BEHAVIORS PLAY ON POCKET</t>
+  </si>
+  <si>
+    <t>PATTERNS POSITIONAL.IMPROVING TECHNICAL/TACTICAL &amp; CROSS + FINISIHING</t>
+  </si>
+  <si>
+    <t>POST MATCH WBA. AVOID LOSSES</t>
+  </si>
+  <si>
+    <t>OPPONENT COVENTRY</t>
+  </si>
+  <si>
+    <t>PERSONAL INTERVIEW. U20</t>
+  </si>
+  <si>
+    <t>COUNTER ATTACK &amp; FINISHING. 1vs1 (GK)</t>
+  </si>
+  <si>
+    <t>COMPETITIVE FINISHING DRILLS</t>
+  </si>
+  <si>
+    <t>TRAINING NON SQUAD. OFFENSIVE PATTERNS &amp; FINISHING</t>
+  </si>
+  <si>
+    <t>DEFENDER ONE-TWO. BUILD UP CONNECTED WITH 11/9</t>
+  </si>
+  <si>
+    <t>DEFENDER ONE-TWO. BUILD UP CONNECTED WITH 7/9</t>
+  </si>
+  <si>
+    <t>IMPROVING CROSSES 1st POST &amp; 2nd POST</t>
+  </si>
+  <si>
+    <t>ATTACK ON THE BOX &amp; FINISHING</t>
   </si>
 </sst>
 </file>
@@ -1328,10 +1388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D1F4C8-8FC1-6D4C-8100-17BA8EC0B4E7}">
-  <dimension ref="A1:F722"/>
+  <dimension ref="A1:F797"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A707" workbookViewId="0">
-      <selection activeCell="D725" sqref="D725"/>
+    <sheetView tabSelected="1" topLeftCell="A773" workbookViewId="0">
+      <selection activeCell="C804" sqref="C804"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7474,7 +7534,7 @@
       <c r="B544" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D544" t="s">
+      <c r="E544" t="s">
         <v>253</v>
       </c>
     </row>
@@ -7584,7 +7644,7 @@
       <c r="B554" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D554" t="s">
+      <c r="E554" t="s">
         <v>253</v>
       </c>
     </row>
@@ -7897,7 +7957,7 @@
       <c r="B583" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D583" t="s">
+      <c r="E583" t="s">
         <v>247</v>
       </c>
     </row>
@@ -7908,7 +7968,7 @@
       <c r="B584" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D584" t="s">
+      <c r="E584" t="s">
         <v>247</v>
       </c>
     </row>
@@ -9431,6 +9491,831 @@
       </c>
       <c r="C722" t="s">
         <v>288</v>
+      </c>
+    </row>
+    <row r="723" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A723" s="1">
+        <v>45945</v>
+      </c>
+      <c r="B723" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C723" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="724" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A724" s="1">
+        <v>45945</v>
+      </c>
+      <c r="B724" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C724" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="725" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A725" s="1">
+        <v>45945</v>
+      </c>
+      <c r="B725" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C725" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="726" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A726" s="1">
+        <v>45945</v>
+      </c>
+      <c r="B726" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C726" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="727" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A727" s="1">
+        <v>45945</v>
+      </c>
+      <c r="B727" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C727" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="728" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A728" s="1">
+        <v>45945</v>
+      </c>
+      <c r="B728" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C728" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="729" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A729" s="1">
+        <v>45945</v>
+      </c>
+      <c r="B729" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C729" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="730" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A730" s="1">
+        <v>45946</v>
+      </c>
+      <c r="B730" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C730" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="731" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A731" s="1">
+        <v>45946</v>
+      </c>
+      <c r="B731" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C731" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="732" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A732" s="1">
+        <v>45946</v>
+      </c>
+      <c r="B732" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C732" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="733" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A733" s="1">
+        <v>45946</v>
+      </c>
+      <c r="B733" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C733" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="734" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A734" s="1">
+        <v>45946</v>
+      </c>
+      <c r="B734" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C734" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="735" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A735" s="1">
+        <v>45946</v>
+      </c>
+      <c r="B735" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C735" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="736" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A736" s="1">
+        <v>45947</v>
+      </c>
+      <c r="B736" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C736" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="737" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A737" s="1">
+        <v>45949</v>
+      </c>
+      <c r="B737" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C737" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="738" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A738" s="1">
+        <v>45949</v>
+      </c>
+      <c r="B738" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C738" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="739" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A739" s="1">
+        <v>45949</v>
+      </c>
+      <c r="B739" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C739" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="740" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A740" s="1">
+        <v>45949</v>
+      </c>
+      <c r="B740" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C740" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="741" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A741" s="1">
+        <v>45949</v>
+      </c>
+      <c r="B741" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C741" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="742" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A742" s="1">
+        <v>45949</v>
+      </c>
+      <c r="B742" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C742" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="743" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A743" s="1">
+        <v>45950</v>
+      </c>
+      <c r="B743" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C743" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="744" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A744" s="1">
+        <v>45950</v>
+      </c>
+      <c r="B744" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C744" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="745" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A745" s="1">
+        <v>45950</v>
+      </c>
+      <c r="B745" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C745" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="746" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A746" s="1">
+        <v>45950</v>
+      </c>
+      <c r="B746" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E746" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="747" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A747" s="1">
+        <v>45951</v>
+      </c>
+      <c r="B747" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E747" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="748" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A748" s="1">
+        <v>45952</v>
+      </c>
+      <c r="B748" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C748" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="749" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A749" s="1">
+        <v>45952</v>
+      </c>
+      <c r="B749" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C749" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="750" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A750" s="1">
+        <v>45952</v>
+      </c>
+      <c r="B750" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C750" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="751" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A751" s="1">
+        <v>45952</v>
+      </c>
+      <c r="B751" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C751" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="752" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A752" s="1">
+        <v>45952</v>
+      </c>
+      <c r="B752" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C752" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="753" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A753" s="1">
+        <v>45953</v>
+      </c>
+      <c r="B753" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E753" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="754" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A754" s="1">
+        <v>45954</v>
+      </c>
+      <c r="B754" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E754" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="755" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A755" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B755" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C755" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="756" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A756" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B756" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C756" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="757" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A757" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B757" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C757" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="758" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A758" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B758" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C758" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="759" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A759" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B759" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C759" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="760" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A760" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B760" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C760" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="761" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A761" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B761" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C761" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="762" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A762" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B762" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C762" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="763" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A763" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B763" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C763" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="764" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A764" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B764" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C764" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="765" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A765" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B765" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C765" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="766" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A766" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B766" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C766" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="767" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A767" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B767" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C767" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="768" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A768" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B768" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C768" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="769" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A769" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B769" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C769" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="770" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A770" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B770" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C770" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="771" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A771" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B771" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D771" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="772" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A772" s="1">
+        <v>45960</v>
+      </c>
+      <c r="B772" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C772" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="773" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A773" s="1">
+        <v>45960</v>
+      </c>
+      <c r="B773" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C773" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="774" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A774" s="1">
+        <v>45960</v>
+      </c>
+      <c r="B774" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C774" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="775" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A775" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B775" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C775" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="776" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A776" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B776" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C776" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="777" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A777" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B777" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C777" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="778" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A778" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B778" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C778" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="779" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A779" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B779" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C779" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="780" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A780" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B780" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C780" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="781" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A781" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B781" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C781" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="782" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A782" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B782" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C782" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="783" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A783" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B783" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C783" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="784" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A784" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B784" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C784" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="785" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A785" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B785" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C785" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="786" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A786" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B786" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C786" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="787" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A787" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B787" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C787" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="788" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A788" s="1">
+        <v>45962</v>
+      </c>
+      <c r="B788" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C788" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="789" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A789" s="1">
+        <v>45962</v>
+      </c>
+      <c r="B789" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C789" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="790" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A790" s="1">
+        <v>45962</v>
+      </c>
+      <c r="B790" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C790" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="791" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A791" s="1">
+        <v>45962</v>
+      </c>
+      <c r="B791" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C791" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="792" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A792" s="1">
+        <v>45964</v>
+      </c>
+      <c r="B792" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C792" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="793" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A793" s="1">
+        <v>45964</v>
+      </c>
+      <c r="B793" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C793" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="794" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A794" s="1">
+        <v>45966</v>
+      </c>
+      <c r="B794" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C794" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="795" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A795" s="1">
+        <v>45966</v>
+      </c>
+      <c r="B795" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C795" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="796" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A796" s="1">
+        <v>45966</v>
+      </c>
+      <c r="B796" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C796" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="797" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A797" s="1">
+        <v>45966</v>
+      </c>
+      <c r="B797" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C797" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>